<commit_message>
final backbone of backend. Some minor checks left
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -73,25 +73,52 @@
     <t xml:space="preserve">Home State</t>
   </si>
   <si>
-    <t xml:space="preserve">Ansh Mehrotra</t>
+    <t xml:space="preserve">Ansh zehrotra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CS28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">211339</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imehrotraansh02@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8299545361</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9855+39695</t>
+  </si>
+  <si>
+    <t xml:space="preserve">526352</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2636256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5263626</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">852852</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neeraj Mehrotra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bczs</t>
   </si>
   <si>
     <t xml:space="preserve">CS78</t>
   </si>
   <si>
     <t xml:space="preserve">CSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">imehrotraansh02@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9855+39695</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bczs</t>
   </si>
   <si>
     <t xml:space="preserve">211360@juitsolan.in</t>
@@ -114,7 +141,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,12 +170,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -205,15 +226,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -411,174 +432,165 @@
   </sheetPr>
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P7" activeCellId="0" sqref="P7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q9" activeCellId="0" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="26.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="12.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="11.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>211339</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>2025</v>
-      </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="3" t="n">
         <v>37804</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="0" t="n">
-        <v>8299545361</v>
-      </c>
-      <c r="J2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="0" t="n">
-        <v>526352</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>2636256</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <v>5263626</v>
-      </c>
-      <c r="N2" s="0" t="n">
-        <v>52322</v>
-      </c>
-      <c r="O2" s="0" t="n">
-        <v>852852</v>
-      </c>
-      <c r="P2" s="0" t="n">
-        <v>2365358</v>
-      </c>
-      <c r="Q2" s="0" t="n">
-        <v>0</v>
+      <c r="J2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>211360</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="0" t="n">
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="1" t="n">
         <v>1234567890</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="0" t="n">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>211307</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="0" t="n">
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="1" t="n">
         <v>8840563865</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add images folder in static and added juit logo here
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -618,7 +618,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2113259</t>
+          <t>211339</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>btech</t>
+          <t>bth</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -656,7 +656,11 @@
           <t>imehrotraansh02@gmail.com</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>1411414444</t>
@@ -682,28 +686,100 @@
           <t>afFFAFA</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="inlineStr"/>
-      <c r="AD2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="AE2" t="inlineStr"/>
-      <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="inlineStr"/>
-      <c r="AH2" t="inlineStr"/>
-      <c r="AI2" t="inlineStr"/>
-      <c r="AJ2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">

</xml_diff>

<commit_message>
ADDED DROPDOWN IN JOINING YEAR AND PASSOUT YEAR
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -618,7 +618,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>211339</t>
+          <t xml:space="preserve">211339 </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">

</xml_diff>